<commit_message>
BUG instruction images not showing
</commit_message>
<xml_diff>
--- a/schedules/3_Extinction.xlsx.xlsx
+++ b/schedules/3_Extinction.xlsx.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="PreCond" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="RatingPreCond" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PreCond1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1239,8 +1240,6 @@
       <c r="B3" t="n">
         <v>0.4</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
         <v>1</v>
       </c>
@@ -1345,8 +1344,6 @@
       <c r="B4" t="n">
         <v>0.6</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>1</v>
       </c>
@@ -1469,8 +1466,6 @@
       <c r="B5" t="n">
         <v>0.9</v>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
         <v>1</v>
       </c>
@@ -1653,6 +1648,1021 @@
       </c>
       <c r="B14" t="n">
         <v>60.0052084522415</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>PreCondName</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TrgCol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>PreCondTriggKey.keys_raw</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>PreCondTriggMouse.leftButton_raw</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>PreCondTriggMouse.midButton_raw</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>PreCondTriggMouse.rightButton_raw</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>PreCondTriggMouse.time_raw</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>PreCondTriggMouse.x_raw</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>PreCondTriggMouse.y_raw</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>stimuli/Neg.BMP</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>stimuli/Neg.BMP</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>stimuli/Neg.BMP</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>stimuli/Neg.BMP</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>stimuli/Neg.BMP</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>stimuli/Neu.BMP</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>stimuli/Neu.BMP</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>stimuli/Neu.BMP</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>stimuli/Neu.BMP</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>stimuli/Neu.BMP</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>stimuli/Pos.BMP</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>stimuli/Pos.BMP</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>stimuli/Pos.BMP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>stimuli/Pos.BMP</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>stimuli/Pos.BMP</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>stimuli/Trig.BMP</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>stimuli/Trig.BMP</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>stimuli/Trig.BMP</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>'--'</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>extraInfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Participant_ID</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>S00dsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Language</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>EN</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2023-06-28_00h05.04.770</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>expName</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>TCET</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>psychopyVersion</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2023.1.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>frameRate</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>59.96296686889758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>